<commit_message>
ft Agregada cláusula para encontrar relaciones
</commit_message>
<xml_diff>
--- a/resources/prueba.xlsx
+++ b/resources/prueba.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="55">
   <si>
     <t xml:space="preserve">Table:</t>
   </si>
@@ -143,6 +143,49 @@
   </si>
   <si>
     <t xml:space="preserve">putcnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relationships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foreign database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foreign table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Join</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relationship name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mainserver_bdicobranza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">informix.cb_campanias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Many to one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">informix.cb_tipos_campanias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id_tipo = informix.cb_tipos_campanias.id_tipo and
+empresa = informix.cb_tipos_campanias.empresa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r117_38</t>
   </si>
 </sst>
 </file>
@@ -157,6 +200,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -223,13 +267,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -355,329 +411,463 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="5.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="32.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="5.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="17.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="17.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="J11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="0" t="s">
+      <c r="K11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="0" t="s">
+      <c r="L11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="0" t="s">
+      <c r="M11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="0" t="s">
+      <c r="N11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O11" s="0" t="s">
+      <c r="O11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P11" s="0" t="s">
+      <c r="P11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="Q11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R11" s="0" t="s">
+      <c r="R11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S11" s="0" t="s">
+      <c r="S11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T11" s="0" t="s">
+      <c r="T11" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" s="0" t="s">
+      <c r="I12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="0" t="s">
+      <c r="I13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J14" s="0" t="s">
+      <c r="I14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I15" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J15" s="0" t="s">
+      <c r="I15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J16" s="0" t="s">
+      <c r="I16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="G17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="0" t="s">
+      <c r="I17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J18" s="0" t="s">
+      <c r="I18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>31</v>
-      </c>
+      <c r="I19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" s="0"/>
+      <c r="I23" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="J23" s="0"/>
+      <c r="K23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="0"/>
+      <c r="I24" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="J24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="0"/>
+      <c r="I25" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="J25" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>